<commit_message>
update on manuscript and main figure1-5
</commit_message>
<xml_diff>
--- a/ID89.signature.summary/ID89_and_ID83.summary-2025-06-05.xlsx
+++ b/ID89.signature.summary/ID89_and_ID83.summary-2025-06-05.xlsx
@@ -5,17 +5,18 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\github2\Liu2024\ID89.signature.summary\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/e9c7212a1ac174da/文档/GitHub/Liu2024/ID89.signature.summary/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{82D0593D-C59D-44C5-87C4-7D80914A37D9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="103" documentId="8_{82D0593D-C59D-44C5-87C4-7D80914A37D9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{AABA9244-29B5-4CAF-86C4-66C149472245}"/>
   <bookViews>
-    <workbookView xWindow="-19725" yWindow="-21720" windowWidth="38640" windowHeight="21240" xr2:uid="{1EAECB79-A789-42D9-86BA-9215C29F9749}"/>
+    <workbookView xWindow="-96" yWindow="-96" windowWidth="18912" windowHeight="11952" activeTab="1" xr2:uid="{1EAECB79-A789-42D9-86BA-9215C29F9749}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
     <sheet name="Sheet2" sheetId="2" r:id="rId2"/>
     <sheet name="Sheet3" sheetId="3" r:id="rId3"/>
+    <sheet name="Sheet6" sheetId="6" r:id="rId4"/>
   </sheets>
   <definedNames>
     <definedName name="_xlnm._FilterDatabase" localSheetId="2" hidden="1">Sheet3!$B$3:$B$12</definedName>
@@ -39,19 +40,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="222" uniqueCount="164">
-  <si>
-    <t>ID89 name</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>corresponding ID83</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>Serena's</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="372" uniqueCount="266">
   <si>
     <t>Comments</t>
     <phoneticPr fontId="1" type="noConversion"/>
@@ -473,10 +462,6 @@
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>Cosine similarity</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
     <t>InD23</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
@@ -604,10 +589,6 @@
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t xml:space="preserve">artefact </t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
     <t>Similar to InD26</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
@@ -644,10 +625,6 @@
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>merged</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
     <t>InD11</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
@@ -657,6 +634,348 @@
   </si>
   <si>
     <t>InsDel4</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>corresponding Indel83</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Indel89 as extracted</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Indel89 in Koh et al., 2025</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Cosine similarity between our extraction and Koh et al</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Artefact according to Koh et al.,2025</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Our extraction split the signature</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>InsDel1a</t>
+  </si>
+  <si>
+    <t>Pancreas::SP107784</t>
+  </si>
+  <si>
+    <t>C_ID1</t>
+  </si>
+  <si>
+    <t>InsDel1b</t>
+  </si>
+  <si>
+    <t>Colon::SP21400</t>
+  </si>
+  <si>
+    <t>InsDel1c</t>
+  </si>
+  <si>
+    <t>Breast::CPCT02010523T</t>
+  </si>
+  <si>
+    <t>InsDel1d</t>
+  </si>
+  <si>
+    <t>Esophagus::SP111054</t>
+  </si>
+  <si>
+    <t>InsDel2a</t>
+  </si>
+  <si>
+    <t>Kidney::SP123975</t>
+  </si>
+  <si>
+    <t>C_ID2</t>
+  </si>
+  <si>
+    <t>InsDel2b</t>
+  </si>
+  <si>
+    <t>Colon::SP96118</t>
+  </si>
+  <si>
+    <t>InsDel2c</t>
+  </si>
+  <si>
+    <t>Breast::CPCT02330076T</t>
+  </si>
+  <si>
+    <t>InsDel3</t>
+  </si>
+  <si>
+    <t>Other::CPCT02020815T</t>
+  </si>
+  <si>
+    <t>C_ID3</t>
+  </si>
+  <si>
+    <t>InsDel4a</t>
+  </si>
+  <si>
+    <t>C_ID4</t>
+  </si>
+  <si>
+    <t>InsDel4b</t>
+  </si>
+  <si>
+    <t>InsDel5a</t>
+  </si>
+  <si>
+    <t>Kidney::SP39298</t>
+  </si>
+  <si>
+    <t>C_ID5</t>
+  </si>
+  <si>
+    <t>InsDel5b</t>
+  </si>
+  <si>
+    <t>InsDel6</t>
+  </si>
+  <si>
+    <t>Ovary::SP62616</t>
+  </si>
+  <si>
+    <t>C_ID6</t>
+  </si>
+  <si>
+    <t>InsDel7</t>
+  </si>
+  <si>
+    <t>Uterus::SP90989</t>
+  </si>
+  <si>
+    <t>InsDel8</t>
+  </si>
+  <si>
+    <t>Breast::SP116365</t>
+  </si>
+  <si>
+    <t>C_ID8</t>
+  </si>
+  <si>
+    <t>InsDel24a</t>
+  </si>
+  <si>
+    <t>Breast::SP2293</t>
+  </si>
+  <si>
+    <t>H_ID24</t>
+  </si>
+  <si>
+    <t>InsDel9</t>
+  </si>
+  <si>
+    <t>Pancreas::SP102617</t>
+  </si>
+  <si>
+    <t>C_ID9</t>
+  </si>
+  <si>
+    <t>InsDel10</t>
+  </si>
+  <si>
+    <t>Other::SP109957</t>
+  </si>
+  <si>
+    <t>C_ID10</t>
+  </si>
+  <si>
+    <t>InsDel11</t>
+  </si>
+  <si>
+    <t>Pancreas::SP77956</t>
+  </si>
+  <si>
+    <t>C_ID11</t>
+  </si>
+  <si>
+    <t>InsDel12</t>
+  </si>
+  <si>
+    <t>Prostate::SP112985</t>
+  </si>
+  <si>
+    <t>C_ID12</t>
+  </si>
+  <si>
+    <t>InsDel13</t>
+  </si>
+  <si>
+    <t>Skin::SP124439</t>
+  </si>
+  <si>
+    <t>C_ID13</t>
+  </si>
+  <si>
+    <t>InsDel14</t>
+  </si>
+  <si>
+    <t>InsDel17</t>
+  </si>
+  <si>
+    <t>C_ID19</t>
+  </si>
+  <si>
+    <t>InsDel18</t>
+  </si>
+  <si>
+    <t>Head::CPCT02070053T</t>
+  </si>
+  <si>
+    <t>C_ID18</t>
+  </si>
+  <si>
+    <t>InsDel19a</t>
+  </si>
+  <si>
+    <t>Bone.SoftTissue::CPCT02020325T</t>
+  </si>
+  <si>
+    <t>InsDel19b</t>
+  </si>
+  <si>
+    <t>Skin::CPCT02340081T</t>
+  </si>
+  <si>
+    <t>InsDel19c</t>
+  </si>
+  <si>
+    <t>Skin::CPCT02050079TII</t>
+  </si>
+  <si>
+    <t>InsDel23</t>
+  </si>
+  <si>
+    <t>Kidney::SP102957</t>
+  </si>
+  <si>
+    <t>C_ID23</t>
+  </si>
+  <si>
+    <t>InsDel24b</t>
+  </si>
+  <si>
+    <t>InsDel25</t>
+  </si>
+  <si>
+    <t>InsDel28</t>
+  </si>
+  <si>
+    <t>InsDel29</t>
+  </si>
+  <si>
+    <t>Skin::SP103894</t>
+  </si>
+  <si>
+    <t>H_ID29</t>
+  </si>
+  <si>
+    <t>InsDel30</t>
+  </si>
+  <si>
+    <t>Other::DRUP01030015T</t>
+  </si>
+  <si>
+    <t>H_ID30</t>
+  </si>
+  <si>
+    <t>InsDel32</t>
+  </si>
+  <si>
+    <t>CNS::SP107439</t>
+  </si>
+  <si>
+    <t>H_ID32</t>
+  </si>
+  <si>
+    <t>InsDel33</t>
+  </si>
+  <si>
+    <t>InsDel34a</t>
+  </si>
+  <si>
+    <t>InsDel34b</t>
+  </si>
+  <si>
+    <t>InsDel35</t>
+  </si>
+  <si>
+    <t>InsDel36</t>
+  </si>
+  <si>
+    <t>Prostate::SP112777</t>
+  </si>
+  <si>
+    <t>H_ID36</t>
+  </si>
+  <si>
+    <t>InsDel38</t>
+  </si>
+  <si>
+    <t>InsDel39</t>
+  </si>
+  <si>
+    <t>Colon::CPCT02010512T</t>
+  </si>
+  <si>
+    <t>Other::CPCT02250003T</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>CNS::SP24135</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>CNS::CPCT02100089T</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Liver::SP112290</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Colon::CPCT02340014T</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Bone.SoftTissue::SP122372</t>
+  </si>
+  <si>
+    <t>Uterus::DRUP01340014T</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Pancreas::SP70106</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Colon::SP17905</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Prostate::SP112817</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>CNS::CPCT02100101T</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Kidney::SP102897</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Breast::DRUP01010037T/Stomach::CPCT02030347T</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
@@ -664,18 +983,18 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="20">
+  <fonts count="21" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
-      <name val="Calibri"/>
+      <name val="等线"/>
       <family val="2"/>
       <charset val="134"/>
       <scheme val="minor"/>
     </font>
     <font>
       <sz val="9"/>
-      <name val="Calibri"/>
+      <name val="等线"/>
       <family val="2"/>
       <charset val="134"/>
       <scheme val="minor"/>
@@ -683,14 +1002,14 @@
     <font>
       <sz val="12"/>
       <color theme="1"/>
-      <name val="Calibri"/>
+      <name val="等线"/>
       <family val="2"/>
       <scheme val="minor"/>
     </font>
     <font>
       <sz val="18"/>
       <color theme="3"/>
-      <name val="Calibri Light"/>
+      <name val="等线 Light"/>
       <family val="2"/>
       <scheme val="major"/>
     </font>
@@ -698,7 +1017,7 @@
       <b/>
       <sz val="15"/>
       <color theme="3"/>
-      <name val="Calibri"/>
+      <name val="等线"/>
       <family val="2"/>
       <scheme val="minor"/>
     </font>
@@ -706,7 +1025,7 @@
       <b/>
       <sz val="13"/>
       <color theme="3"/>
-      <name val="Calibri"/>
+      <name val="等线"/>
       <family val="2"/>
       <scheme val="minor"/>
     </font>
@@ -714,35 +1033,35 @@
       <b/>
       <sz val="11"/>
       <color theme="3"/>
-      <name val="Calibri"/>
+      <name val="等线"/>
       <family val="2"/>
       <scheme val="minor"/>
     </font>
     <font>
       <sz val="12"/>
       <color rgb="FF006100"/>
-      <name val="Calibri"/>
+      <name val="等线"/>
       <family val="2"/>
       <scheme val="minor"/>
     </font>
     <font>
       <sz val="12"/>
       <color rgb="FF9C0006"/>
-      <name val="Calibri"/>
+      <name val="等线"/>
       <family val="2"/>
       <scheme val="minor"/>
     </font>
     <font>
       <sz val="12"/>
       <color rgb="FF9C5700"/>
-      <name val="Calibri"/>
+      <name val="等线"/>
       <family val="2"/>
       <scheme val="minor"/>
     </font>
     <font>
       <sz val="12"/>
       <color rgb="FF3F3F76"/>
-      <name val="Calibri"/>
+      <name val="等线"/>
       <family val="2"/>
       <scheme val="minor"/>
     </font>
@@ -750,7 +1069,7 @@
       <b/>
       <sz val="12"/>
       <color rgb="FF3F3F3F"/>
-      <name val="Calibri"/>
+      <name val="等线"/>
       <family val="2"/>
       <scheme val="minor"/>
     </font>
@@ -758,14 +1077,14 @@
       <b/>
       <sz val="12"/>
       <color rgb="FFFA7D00"/>
-      <name val="Calibri"/>
+      <name val="等线"/>
       <family val="2"/>
       <scheme val="minor"/>
     </font>
     <font>
       <sz val="12"/>
       <color rgb="FFFA7D00"/>
-      <name val="Calibri"/>
+      <name val="等线"/>
       <family val="2"/>
       <scheme val="minor"/>
     </font>
@@ -773,14 +1092,14 @@
       <b/>
       <sz val="12"/>
       <color theme="0"/>
-      <name val="Calibri"/>
+      <name val="等线"/>
       <family val="2"/>
       <scheme val="minor"/>
     </font>
     <font>
       <sz val="12"/>
       <color rgb="FFFF0000"/>
-      <name val="Calibri"/>
+      <name val="等线"/>
       <family val="2"/>
       <scheme val="minor"/>
     </font>
@@ -788,7 +1107,7 @@
       <i/>
       <sz val="12"/>
       <color rgb="FF7F7F7F"/>
-      <name val="Calibri"/>
+      <name val="等线"/>
       <family val="2"/>
       <scheme val="minor"/>
     </font>
@@ -796,14 +1115,14 @@
       <b/>
       <sz val="12"/>
       <color theme="1"/>
-      <name val="Calibri"/>
+      <name val="等线"/>
       <family val="2"/>
       <scheme val="minor"/>
     </font>
     <font>
       <sz val="12"/>
       <color theme="0"/>
-      <name val="Calibri"/>
+      <name val="等线"/>
       <family val="2"/>
       <scheme val="minor"/>
     </font>
@@ -812,6 +1131,12 @@
       <color rgb="FF586E75"/>
       <name val="Cascadia Code"/>
       <family val="3"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <color rgb="FF586E75"/>
+      <name val="Segoe UI"/>
+      <family val="2"/>
     </font>
   </fonts>
   <fills count="37">
@@ -1182,7 +1507,7 @@
     <xf numFmtId="0" fontId="2" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="7">
+  <cellXfs count="9">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
       <alignment vertical="center"/>
     </xf>
@@ -1202,6 +1527,12 @@
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="34" borderId="0" xfId="0" applyFont="1" applyFill="1">
+      <alignment vertical="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="43">
     <cellStyle name="20% - Accent1 2" xfId="20" xr:uid="{96642AB3-9DEB-44DC-BE63-718714B165A9}"/>
@@ -1262,9 +1593,9 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office 2013 - 2022 Theme">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
   <a:themeElements>
-    <a:clrScheme name="Office 2013 - 2022">
+    <a:clrScheme name="Office">
       <a:dk1>
         <a:sysClr val="windowText" lastClr="000000"/>
       </a:dk1>
@@ -1302,7 +1633,7 @@
         <a:srgbClr val="954F72"/>
       </a:folHlink>
     </a:clrScheme>
-    <a:fontScheme name="Office 2013 - 2022">
+    <a:fontScheme name="Office">
       <a:majorFont>
         <a:latin typeface="Calibri Light" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
@@ -1408,7 +1739,7 @@
         <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
-    <a:fmtScheme name="Office 2013 - 2022">
+    <a:fmtScheme name="Office">
       <a:fillStyleLst>
         <a:solidFill>
           <a:schemeClr val="phClr"/>
@@ -1550,7 +1881,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office 2013 - 2022 Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -1560,526 +1891,525 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E1986EDA-ED44-411B-A31B-549A3D83E29F}">
   <dimension ref="A1:E46"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C1" sqref="C1"/>
-    </sheetView>
+    <sheetView topLeftCell="A25" workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4"/>
+  <sheetFormatPr defaultRowHeight="14.1" x14ac:dyDescent="0.5"/>
   <cols>
-    <col min="1" max="1" width="9.5546875" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="16.88671875" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="13.88671875" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="23.88671875" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="29.19921875" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="20.94921875" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="23.546875" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="19.94921875" customWidth="1"/>
+    <col min="5" max="5" width="23.8984375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5">
+    <row r="1" spans="1:5" ht="56.4" x14ac:dyDescent="0.5">
       <c r="A1" t="s">
+        <v>159</v>
+      </c>
+      <c r="B1" t="s">
+        <v>158</v>
+      </c>
+      <c r="C1" t="s">
+        <v>160</v>
+      </c>
+      <c r="D1" s="7" t="s">
+        <v>161</v>
+      </c>
+      <c r="E1" t="s">
         <v>0</v>
       </c>
-      <c r="B1" t="s">
-        <v>1</v>
-      </c>
-      <c r="C1" t="s">
-        <v>2</v>
-      </c>
-      <c r="D1" t="s">
-        <v>108</v>
-      </c>
-      <c r="E1" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="2" spans="1:5">
+    </row>
+    <row r="2" spans="1:5" x14ac:dyDescent="0.5">
       <c r="A2" t="s">
-        <v>19</v>
+        <v>16</v>
       </c>
       <c r="B2" t="s">
-        <v>18</v>
+        <v>15</v>
       </c>
       <c r="C2" t="s">
-        <v>98</v>
+        <v>95</v>
       </c>
       <c r="D2">
         <v>0.96</v>
       </c>
       <c r="E2" t="s">
-        <v>22</v>
-      </c>
-    </row>
-    <row r="3" spans="1:5">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5" x14ac:dyDescent="0.5">
       <c r="A3" t="s">
-        <v>20</v>
+        <v>17</v>
       </c>
       <c r="B3" t="s">
-        <v>18</v>
+        <v>15</v>
       </c>
       <c r="C3" t="s">
-        <v>99</v>
+        <v>96</v>
       </c>
       <c r="D3">
         <v>0.96</v>
       </c>
       <c r="E3" t="s">
-        <v>21</v>
-      </c>
-    </row>
-    <row r="4" spans="1:5">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5" x14ac:dyDescent="0.5">
       <c r="A4" t="s">
-        <v>36</v>
+        <v>33</v>
       </c>
       <c r="B4" t="s">
-        <v>18</v>
+        <v>15</v>
       </c>
       <c r="C4" t="s">
-        <v>100</v>
+        <v>97</v>
       </c>
       <c r="D4">
         <v>0.91</v>
       </c>
     </row>
-    <row r="5" spans="1:5">
+    <row r="5" spans="1:5" x14ac:dyDescent="0.5">
       <c r="A5" t="s">
-        <v>78</v>
+        <v>75</v>
       </c>
       <c r="B5" t="s">
-        <v>18</v>
+        <v>15</v>
       </c>
       <c r="E5" t="s">
-        <v>79</v>
-      </c>
-    </row>
-    <row r="6" spans="1:5">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="6" spans="1:5" x14ac:dyDescent="0.5">
       <c r="A6" t="s">
-        <v>6</v>
+        <v>3</v>
       </c>
       <c r="B6" t="s">
-        <v>7</v>
+        <v>4</v>
       </c>
       <c r="C6" t="s">
-        <v>76</v>
+        <v>73</v>
       </c>
       <c r="D6">
         <v>0.99</v>
       </c>
     </row>
-    <row r="7" spans="1:5">
+    <row r="7" spans="1:5" x14ac:dyDescent="0.5">
       <c r="A7" t="s">
-        <v>11</v>
+        <v>8</v>
       </c>
       <c r="B7" t="s">
-        <v>7</v>
+        <v>4</v>
       </c>
       <c r="E7" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="8" spans="1:5">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="8" spans="1:5" x14ac:dyDescent="0.5">
       <c r="A8" t="s">
-        <v>44</v>
+        <v>41</v>
       </c>
       <c r="B8" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="9" spans="1:5">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="9" spans="1:5" x14ac:dyDescent="0.5">
       <c r="A9" t="s">
-        <v>4</v>
+        <v>1</v>
       </c>
       <c r="B9" t="s">
-        <v>5</v>
+        <v>2</v>
       </c>
       <c r="C9" t="s">
-        <v>95</v>
+        <v>92</v>
       </c>
       <c r="D9">
         <v>0.94</v>
       </c>
     </row>
-    <row r="10" spans="1:5">
+    <row r="10" spans="1:5" x14ac:dyDescent="0.5">
       <c r="A10" t="s">
-        <v>81</v>
+        <v>78</v>
       </c>
       <c r="B10" t="s">
-        <v>28</v>
+        <v>25</v>
       </c>
       <c r="C10" t="s">
-        <v>29</v>
+        <v>26</v>
       </c>
       <c r="D10">
         <v>0.97</v>
       </c>
     </row>
-    <row r="11" spans="1:5">
+    <row r="11" spans="1:5" x14ac:dyDescent="0.5">
       <c r="A11" t="s">
-        <v>50</v>
+        <v>47</v>
       </c>
       <c r="B11" t="s">
-        <v>28</v>
+        <v>25</v>
       </c>
       <c r="E11" t="s">
-        <v>51</v>
-      </c>
-    </row>
-    <row r="12" spans="1:5">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="12" spans="1:5" x14ac:dyDescent="0.5">
       <c r="A12" t="s">
-        <v>25</v>
+        <v>22</v>
       </c>
       <c r="B12" t="s">
-        <v>26</v>
+        <v>23</v>
       </c>
       <c r="C12" t="s">
-        <v>27</v>
+        <v>24</v>
       </c>
       <c r="E12" t="s">
-        <v>40</v>
-      </c>
-    </row>
-    <row r="13" spans="1:5">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="13" spans="1:5" x14ac:dyDescent="0.5">
       <c r="A13" t="s">
-        <v>38</v>
+        <v>35</v>
       </c>
       <c r="B13" t="s">
-        <v>26</v>
+        <v>23</v>
       </c>
       <c r="E13" t="s">
-        <v>39</v>
-      </c>
-    </row>
-    <row r="14" spans="1:5">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="14" spans="1:5" x14ac:dyDescent="0.5">
       <c r="A14" t="s">
-        <v>12</v>
+        <v>9</v>
       </c>
       <c r="B14" t="s">
-        <v>13</v>
+        <v>10</v>
       </c>
       <c r="C14" t="s">
-        <v>77</v>
+        <v>74</v>
       </c>
       <c r="D14">
         <v>0.98</v>
       </c>
     </row>
-    <row r="15" spans="1:5">
+    <row r="15" spans="1:5" x14ac:dyDescent="0.5">
       <c r="A15" t="s">
-        <v>74</v>
+        <v>71</v>
       </c>
       <c r="B15" t="s">
-        <v>75</v>
+        <v>72</v>
       </c>
       <c r="C15" t="s">
-        <v>80</v>
+        <v>77</v>
       </c>
       <c r="D15">
         <v>0.97</v>
       </c>
     </row>
-    <row r="16" spans="1:5">
+    <row r="16" spans="1:5" x14ac:dyDescent="0.5">
       <c r="A16" t="s">
-        <v>30</v>
+        <v>27</v>
       </c>
       <c r="B16" t="s">
-        <v>31</v>
+        <v>28</v>
       </c>
       <c r="C16" t="s">
-        <v>32</v>
+        <v>29</v>
       </c>
       <c r="D16">
         <v>0.95</v>
       </c>
     </row>
-    <row r="17" spans="1:5">
+    <row r="17" spans="1:5" x14ac:dyDescent="0.5">
       <c r="A17" t="s">
-        <v>9</v>
+        <v>6</v>
       </c>
       <c r="B17" t="s">
-        <v>10</v>
+        <v>7</v>
       </c>
       <c r="C17" t="s">
-        <v>96</v>
+        <v>93</v>
       </c>
       <c r="D17">
         <v>0.92</v>
       </c>
     </row>
-    <row r="18" spans="1:5">
+    <row r="18" spans="1:5" x14ac:dyDescent="0.5">
       <c r="A18" t="s">
-        <v>23</v>
+        <v>20</v>
       </c>
       <c r="B18" t="s">
-        <v>10</v>
+        <v>7</v>
       </c>
       <c r="C18" t="s">
-        <v>24</v>
+        <v>21</v>
       </c>
       <c r="D18">
         <v>0.92</v>
       </c>
     </row>
-    <row r="19" spans="1:5">
+    <row r="19" spans="1:5" x14ac:dyDescent="0.5">
       <c r="A19" t="s">
-        <v>61</v>
+        <v>58</v>
       </c>
       <c r="B19" t="s">
-        <v>60</v>
+        <v>57</v>
       </c>
       <c r="C19" t="s">
-        <v>109</v>
+        <v>105</v>
       </c>
       <c r="D19">
         <v>0.88</v>
       </c>
     </row>
-    <row r="20" spans="1:5">
+    <row r="20" spans="1:5" x14ac:dyDescent="0.5">
       <c r="A20" t="s">
-        <v>62</v>
+        <v>59</v>
       </c>
       <c r="B20" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="21" spans="1:5" x14ac:dyDescent="0.5">
+      <c r="A21" t="s">
+        <v>40</v>
+      </c>
+      <c r="B21" t="s">
         <v>63</v>
       </c>
     </row>
-    <row r="21" spans="1:5">
-      <c r="A21" t="s">
-        <v>43</v>
-      </c>
-      <c r="B21" t="s">
-        <v>66</v>
-      </c>
-    </row>
-    <row r="22" spans="1:5">
+    <row r="22" spans="1:5" x14ac:dyDescent="0.5">
       <c r="A22" t="s">
-        <v>37</v>
+        <v>34</v>
       </c>
       <c r="B22" t="s">
-        <v>82</v>
+        <v>79</v>
       </c>
       <c r="C22" t="s">
-        <v>110</v>
+        <v>106</v>
       </c>
       <c r="D22">
         <v>0.99</v>
       </c>
     </row>
-    <row r="23" spans="1:5">
+    <row r="23" spans="1:5" x14ac:dyDescent="0.5">
       <c r="A23" t="s">
-        <v>97</v>
+        <v>94</v>
       </c>
       <c r="B23" t="s">
-        <v>87</v>
+        <v>84</v>
       </c>
       <c r="C23" t="s">
-        <v>101</v>
+        <v>98</v>
       </c>
       <c r="D23">
         <v>0.98</v>
       </c>
       <c r="E23" t="s">
-        <v>86</v>
-      </c>
-    </row>
-    <row r="24" spans="1:5">
+        <v>83</v>
+      </c>
+    </row>
+    <row r="24" spans="1:5" x14ac:dyDescent="0.5">
       <c r="A24" t="s">
-        <v>52</v>
+        <v>49</v>
       </c>
       <c r="B24" t="s">
-        <v>53</v>
-      </c>
-    </row>
-    <row r="25" spans="1:5">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="25" spans="1:5" x14ac:dyDescent="0.5">
       <c r="A25" t="s">
-        <v>45</v>
+        <v>42</v>
       </c>
       <c r="B25" t="s">
-        <v>46</v>
+        <v>43</v>
       </c>
       <c r="C25" t="s">
-        <v>47</v>
+        <v>44</v>
       </c>
       <c r="D25">
         <v>0.99</v>
       </c>
     </row>
-    <row r="26" spans="1:5">
+    <row r="26" spans="1:5" x14ac:dyDescent="0.5">
       <c r="A26" t="s">
+        <v>11</v>
+      </c>
+      <c r="B26" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="27" spans="1:5" x14ac:dyDescent="0.5">
+      <c r="A27" t="s">
+        <v>13</v>
+      </c>
+      <c r="B27" t="s">
+        <v>12</v>
+      </c>
+      <c r="E27" t="s">
         <v>14</v>
       </c>
-      <c r="B26" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="27" spans="1:5">
-      <c r="A27" t="s">
-        <v>16</v>
-      </c>
-      <c r="B27" t="s">
-        <v>15</v>
-      </c>
-      <c r="E27" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="28" spans="1:5">
+    </row>
+    <row r="28" spans="1:5" x14ac:dyDescent="0.5">
       <c r="A28" t="s">
-        <v>73</v>
+        <v>70</v>
       </c>
       <c r="B28" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="29" spans="1:5">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="29" spans="1:5" x14ac:dyDescent="0.5">
       <c r="A29" t="s">
-        <v>83</v>
+        <v>80</v>
       </c>
       <c r="B29" t="s">
-        <v>84</v>
-      </c>
-    </row>
-    <row r="30" spans="1:5">
+        <v>81</v>
+      </c>
+    </row>
+    <row r="30" spans="1:5" x14ac:dyDescent="0.5">
       <c r="A30" t="s">
+        <v>51</v>
+      </c>
+      <c r="B30" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="31" spans="1:5" x14ac:dyDescent="0.5">
+      <c r="A31" t="s">
+        <v>103</v>
+      </c>
+      <c r="B31" t="s">
+        <v>101</v>
+      </c>
+    </row>
+    <row r="32" spans="1:5" x14ac:dyDescent="0.5">
+      <c r="A32" t="s">
+        <v>55</v>
+      </c>
+      <c r="B32" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="33" spans="1:5" x14ac:dyDescent="0.5">
+      <c r="A33" t="s">
+        <v>30</v>
+      </c>
+      <c r="B33" t="s">
+        <v>31</v>
+      </c>
+      <c r="E33" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="34" spans="1:5" x14ac:dyDescent="0.5">
+      <c r="A34" t="s">
+        <v>38</v>
+      </c>
+      <c r="B34" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="35" spans="1:5" x14ac:dyDescent="0.5">
+      <c r="A35" t="s">
+        <v>88</v>
+      </c>
+      <c r="B35" t="s">
+        <v>89</v>
+      </c>
+    </row>
+    <row r="36" spans="1:5" x14ac:dyDescent="0.5">
+      <c r="A36" t="s">
+        <v>86</v>
+      </c>
+      <c r="B36" t="s">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="37" spans="1:5" x14ac:dyDescent="0.5">
+      <c r="A37" t="s">
+        <v>53</v>
+      </c>
+      <c r="B37" t="s">
         <v>54</v>
       </c>
-      <c r="B30" t="s">
-        <v>55</v>
-      </c>
-    </row>
-    <row r="31" spans="1:5">
-      <c r="A31" t="s">
-        <v>106</v>
-      </c>
-      <c r="B31" t="s">
-        <v>104</v>
-      </c>
-    </row>
-    <row r="32" spans="1:5">
-      <c r="A32" t="s">
-        <v>58</v>
-      </c>
-      <c r="B32" t="s">
-        <v>59</v>
-      </c>
-    </row>
-    <row r="33" spans="1:5">
-      <c r="A33" t="s">
-        <v>33</v>
-      </c>
-      <c r="B33" t="s">
-        <v>34</v>
-      </c>
-      <c r="E33" t="s">
-        <v>35</v>
-      </c>
-    </row>
-    <row r="34" spans="1:5">
-      <c r="A34" t="s">
-        <v>41</v>
-      </c>
-      <c r="B34" t="s">
-        <v>42</v>
-      </c>
-    </row>
-    <row r="35" spans="1:5">
-      <c r="A35" t="s">
-        <v>91</v>
-      </c>
-      <c r="B35" t="s">
-        <v>92</v>
-      </c>
-    </row>
-    <row r="36" spans="1:5">
-      <c r="A36" t="s">
-        <v>89</v>
-      </c>
-      <c r="B36" t="s">
-        <v>90</v>
-      </c>
-    </row>
-    <row r="37" spans="1:5">
-      <c r="A37" t="s">
-        <v>56</v>
-      </c>
-      <c r="B37" t="s">
-        <v>57</v>
-      </c>
       <c r="E37" t="s">
-        <v>70</v>
-      </c>
-    </row>
-    <row r="38" spans="1:5">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="38" spans="1:5" x14ac:dyDescent="0.5">
       <c r="A38" t="s">
-        <v>71</v>
+        <v>68</v>
       </c>
       <c r="B38" t="s">
-        <v>57</v>
+        <v>54</v>
       </c>
       <c r="E38" t="s">
-        <v>72</v>
-      </c>
-    </row>
-    <row r="39" spans="1:5">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="39" spans="1:5" x14ac:dyDescent="0.5">
       <c r="A39" t="s">
-        <v>64</v>
+        <v>61</v>
       </c>
       <c r="B39" t="s">
-        <v>65</v>
+        <v>62</v>
       </c>
       <c r="C39" t="s">
-        <v>102</v>
+        <v>99</v>
       </c>
       <c r="D39">
         <v>0.97</v>
       </c>
     </row>
-    <row r="40" spans="1:5">
+    <row r="40" spans="1:5" x14ac:dyDescent="0.5">
       <c r="A40" t="s">
-        <v>68</v>
+        <v>65</v>
       </c>
       <c r="B40" t="s">
-        <v>67</v>
+        <v>64</v>
       </c>
       <c r="E40" t="s">
-        <v>69</v>
-      </c>
-    </row>
-    <row r="41" spans="1:5">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="41" spans="1:5" x14ac:dyDescent="0.5">
       <c r="A41" t="s">
-        <v>48</v>
+        <v>45</v>
       </c>
       <c r="B41" t="s">
-        <v>49</v>
+        <v>46</v>
       </c>
       <c r="C41" t="s">
-        <v>103</v>
+        <v>100</v>
       </c>
       <c r="D41">
         <v>0.93</v>
       </c>
       <c r="E41" t="s">
-        <v>111</v>
-      </c>
-    </row>
-    <row r="42" spans="1:5">
+        <v>107</v>
+      </c>
+    </row>
+    <row r="42" spans="1:5" x14ac:dyDescent="0.5">
       <c r="A42" t="s">
+        <v>82</v>
+      </c>
+    </row>
+    <row r="44" spans="1:5" x14ac:dyDescent="0.5">
+      <c r="A44" t="s">
+        <v>104</v>
+      </c>
+    </row>
+    <row r="45" spans="1:5" x14ac:dyDescent="0.5">
+      <c r="B45" t="s">
         <v>85</v>
       </c>
-    </row>
-    <row r="44" spans="1:5">
-      <c r="A44" t="s">
-        <v>107</v>
-      </c>
-    </row>
-    <row r="45" spans="1:5">
-      <c r="B45" t="s">
-        <v>88</v>
-      </c>
       <c r="E45" t="s">
-        <v>105</v>
-      </c>
-    </row>
-    <row r="46" spans="1:5">
+        <v>102</v>
+      </c>
+    </row>
+    <row r="46" spans="1:5" x14ac:dyDescent="0.5">
       <c r="B46" t="s">
-        <v>93</v>
+        <v>90</v>
       </c>
       <c r="E46" t="s">
-        <v>94</v>
+        <v>91</v>
       </c>
     </row>
   </sheetData>
@@ -2090,351 +2420,508 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A609C6E4-D419-4D76-BEA7-70168B835FEF}">
-  <dimension ref="A1:AK37"/>
+  <dimension ref="A1:AK38"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="C3" sqref="C3"/>
+    <sheetView tabSelected="1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="B6" sqref="B6"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4"/>
+  <sheetFormatPr defaultRowHeight="14.1" x14ac:dyDescent="0.5"/>
+  <cols>
+    <col min="1" max="1" width="23.546875" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="18.796875" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="44.546875" bestFit="1" customWidth="1"/>
+  </cols>
   <sheetData>
-    <row r="1" spans="1:37" ht="15.6">
+    <row r="1" spans="1:37" x14ac:dyDescent="0.5">
       <c r="A1" t="s">
+        <v>160</v>
+      </c>
+      <c r="B1" t="s">
+        <v>159</v>
+      </c>
+    </row>
+    <row r="2" spans="1:37" ht="15" x14ac:dyDescent="0.5">
+      <c r="A2" t="s">
+        <v>108</v>
+      </c>
+      <c r="B2" t="s">
+        <v>16</v>
+      </c>
+      <c r="C2" s="6"/>
+      <c r="D2" s="6"/>
+      <c r="E2" s="6"/>
+      <c r="F2" s="6"/>
+      <c r="G2" s="6"/>
+      <c r="H2" s="6"/>
+      <c r="I2" s="6"/>
+      <c r="J2" s="6"/>
+      <c r="K2" s="6"/>
+      <c r="L2" s="6"/>
+      <c r="M2" s="6"/>
+      <c r="N2" s="6"/>
+      <c r="O2" s="6"/>
+      <c r="P2" s="6"/>
+      <c r="Q2" s="6"/>
+      <c r="R2" s="6"/>
+      <c r="S2" s="6"/>
+      <c r="T2" s="6"/>
+      <c r="U2" s="6"/>
+      <c r="V2" s="6"/>
+      <c r="W2" s="6"/>
+      <c r="X2" s="6"/>
+      <c r="Y2" s="6"/>
+      <c r="Z2" s="6"/>
+      <c r="AA2" s="6"/>
+      <c r="AB2" s="6"/>
+      <c r="AC2" s="6"/>
+      <c r="AD2" s="6"/>
+      <c r="AE2" s="6"/>
+      <c r="AF2" s="6"/>
+      <c r="AG2" s="6"/>
+      <c r="AH2" s="6"/>
+      <c r="AI2" s="6"/>
+      <c r="AJ2" s="6"/>
+      <c r="AK2" s="6"/>
+    </row>
+    <row r="3" spans="1:37" x14ac:dyDescent="0.5">
+      <c r="A3" t="s">
+        <v>109</v>
+      </c>
+      <c r="B3" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="4" spans="1:37" x14ac:dyDescent="0.5">
+      <c r="A4" t="s">
+        <v>110</v>
+      </c>
+      <c r="B4" s="4" t="s">
+        <v>148</v>
+      </c>
+      <c r="C4" s="4" t="s">
+        <v>148</v>
+      </c>
+      <c r="E4" t="s">
+        <v>149</v>
+      </c>
+    </row>
+    <row r="5" spans="1:37" x14ac:dyDescent="0.5">
+      <c r="A5" t="s">
+        <v>111</v>
+      </c>
+      <c r="B5" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="6" spans="1:37" x14ac:dyDescent="0.5">
+      <c r="A6" t="s">
         <v>112</v>
       </c>
-      <c r="B1" t="s">
-        <v>19</v>
-      </c>
-      <c r="C1" s="6"/>
-      <c r="D1" s="6"/>
-      <c r="E1" s="6"/>
-      <c r="F1" s="6"/>
-      <c r="G1" s="6"/>
-      <c r="H1" s="6"/>
-      <c r="I1" s="6"/>
-      <c r="J1" s="6"/>
-      <c r="K1" s="6"/>
-      <c r="L1" s="6"/>
-      <c r="M1" s="6"/>
-      <c r="N1" s="6"/>
-      <c r="O1" s="6"/>
-      <c r="P1" s="6"/>
-      <c r="Q1" s="6"/>
-      <c r="R1" s="6"/>
-      <c r="S1" s="6"/>
-      <c r="T1" s="6"/>
-      <c r="U1" s="6"/>
-      <c r="V1" s="6"/>
-      <c r="W1" s="6"/>
-      <c r="X1" s="6"/>
-      <c r="Y1" s="6"/>
-      <c r="Z1" s="6"/>
-      <c r="AA1" s="6"/>
-      <c r="AB1" s="6"/>
-      <c r="AC1" s="6"/>
-      <c r="AD1" s="6"/>
-      <c r="AE1" s="6"/>
-      <c r="AF1" s="6"/>
-      <c r="AG1" s="6"/>
-      <c r="AH1" s="6"/>
-      <c r="AI1" s="6"/>
-      <c r="AJ1" s="6"/>
-      <c r="AK1" s="6"/>
-    </row>
-    <row r="2" spans="1:37">
-      <c r="A2" t="s">
+      <c r="B6" s="4" t="s">
+        <v>150</v>
+      </c>
+      <c r="C6" s="4" t="s">
+        <v>150</v>
+      </c>
+    </row>
+    <row r="7" spans="1:37" x14ac:dyDescent="0.5">
+      <c r="A7" t="s">
         <v>113</v>
       </c>
-      <c r="B2" t="s">
+      <c r="B7" t="s">
+        <v>78</v>
+      </c>
+    </row>
+    <row r="8" spans="1:37" x14ac:dyDescent="0.5">
+      <c r="A8" t="s">
+        <v>114</v>
+      </c>
+      <c r="C8" s="1" t="s">
+        <v>145</v>
+      </c>
+    </row>
+    <row r="9" spans="1:37" x14ac:dyDescent="0.5">
+      <c r="A9" t="s">
+        <v>115</v>
+      </c>
+      <c r="C9" s="4" t="s">
+        <v>162</v>
+      </c>
+    </row>
+    <row r="10" spans="1:37" x14ac:dyDescent="0.5">
+      <c r="A10" t="s">
+        <v>116</v>
+      </c>
+      <c r="B10" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="11" spans="1:37" x14ac:dyDescent="0.5">
+      <c r="A11" t="s">
+        <v>117</v>
+      </c>
+      <c r="B11" t="s">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="12" spans="1:37" x14ac:dyDescent="0.5">
+      <c r="A12" t="s">
+        <v>118</v>
+      </c>
+      <c r="B12" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="13" spans="1:37" x14ac:dyDescent="0.5">
+      <c r="A13" t="s">
+        <v>119</v>
+      </c>
+      <c r="B13" t="s">
         <v>6</v>
       </c>
     </row>
-    <row r="3" spans="1:37">
-      <c r="A3" t="s">
-        <v>114</v>
-      </c>
-      <c r="C3" s="4" t="s">
+    <row r="14" spans="1:37" x14ac:dyDescent="0.5">
+      <c r="A14" t="s">
+        <v>120</v>
+      </c>
+      <c r="B14" t="s">
+        <v>20</v>
+      </c>
+      <c r="G14" t="s">
+        <v>151</v>
+      </c>
+      <c r="H14" t="s">
+        <v>17</v>
+      </c>
+      <c r="I14" t="s">
+        <v>3</v>
+      </c>
+      <c r="J14" t="s">
+        <v>68</v>
+      </c>
+      <c r="L14" t="s">
+        <v>152</v>
+      </c>
+      <c r="M14">
+        <v>0.98199999999999998</v>
+      </c>
+    </row>
+    <row r="15" spans="1:37" x14ac:dyDescent="0.5">
+      <c r="A15" t="s">
+        <v>121</v>
+      </c>
+      <c r="C15" s="2" t="s">
+        <v>163</v>
+      </c>
+      <c r="H15">
+        <v>0.43030590000000002</v>
+      </c>
+      <c r="I15">
+        <v>0.12941359999999999</v>
+      </c>
+      <c r="J15">
+        <v>0.44028050000000002</v>
+      </c>
+    </row>
+    <row r="16" spans="1:37" x14ac:dyDescent="0.5">
+      <c r="A16" t="s">
+        <v>122</v>
+      </c>
+      <c r="C16" s="1" t="s">
+        <v>145</v>
+      </c>
+      <c r="G16" t="s">
         <v>153</v>
       </c>
-      <c r="E3" t="s">
+      <c r="H16" t="s">
+        <v>3</v>
+      </c>
+      <c r="I16" t="s">
+        <v>8</v>
+      </c>
+      <c r="J16" t="s">
+        <v>68</v>
+      </c>
+      <c r="M16">
+        <v>0.98299999999999998</v>
+      </c>
+    </row>
+    <row r="17" spans="1:13" x14ac:dyDescent="0.5">
+      <c r="A17" t="s">
+        <v>123</v>
+      </c>
+      <c r="C17" s="2" t="s">
+        <v>163</v>
+      </c>
+      <c r="H17">
+        <v>0.54020354000000004</v>
+      </c>
+      <c r="I17">
+        <v>0.37409509000000002</v>
+      </c>
+      <c r="J17">
+        <v>8.5701319999999998E-2</v>
+      </c>
+    </row>
+    <row r="18" spans="1:13" x14ac:dyDescent="0.5">
+      <c r="A18" t="s">
+        <v>124</v>
+      </c>
+      <c r="B18" t="s">
+        <v>94</v>
+      </c>
+      <c r="G18" t="s">
         <v>154</v>
       </c>
-    </row>
-    <row r="4" spans="1:37">
-      <c r="A4" t="s">
-        <v>115</v>
-      </c>
-      <c r="B4" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="5" spans="1:37">
-      <c r="A5" t="s">
-        <v>116</v>
-      </c>
-      <c r="C5" s="4" t="s">
+      <c r="H18" t="s">
+        <v>17</v>
+      </c>
+      <c r="I18" t="s">
+        <v>3</v>
+      </c>
+      <c r="J18" t="s">
+        <v>8</v>
+      </c>
+      <c r="M18">
+        <v>0.97399999999999998</v>
+      </c>
+    </row>
+    <row r="19" spans="1:13" x14ac:dyDescent="0.5">
+      <c r="A19" t="s">
+        <v>125</v>
+      </c>
+      <c r="B19" t="s">
+        <v>34</v>
+      </c>
+      <c r="H19">
+        <v>0.48259819999999998</v>
+      </c>
+      <c r="I19">
+        <v>0.27442290000000003</v>
+      </c>
+      <c r="J19">
+        <v>0.2429789</v>
+      </c>
+    </row>
+    <row r="20" spans="1:13" x14ac:dyDescent="0.5">
+      <c r="A20" t="s">
+        <v>126</v>
+      </c>
+      <c r="B20" t="s">
+        <v>33</v>
+      </c>
+      <c r="G20" t="s">
+        <v>133</v>
+      </c>
+      <c r="H20" t="s">
+        <v>33</v>
+      </c>
+      <c r="I20" t="s">
+        <v>71</v>
+      </c>
+      <c r="M20">
+        <v>0.97199999999999998</v>
+      </c>
+    </row>
+    <row r="21" spans="1:13" x14ac:dyDescent="0.5">
+      <c r="A21" t="s">
+        <v>127</v>
+      </c>
+      <c r="B21" t="s">
+        <v>17</v>
+      </c>
+      <c r="H21">
+        <v>0.56460290000000002</v>
+      </c>
+      <c r="I21">
+        <v>0.43539709999999998</v>
+      </c>
+    </row>
+    <row r="22" spans="1:13" x14ac:dyDescent="0.5">
+      <c r="A22" t="s">
+        <v>128</v>
+      </c>
+      <c r="C22" s="2" t="s">
+        <v>163</v>
+      </c>
+      <c r="G22" t="s">
         <v>155</v>
       </c>
-    </row>
-    <row r="6" spans="1:37">
-      <c r="A6" t="s">
-        <v>117</v>
-      </c>
-      <c r="B6" t="s">
-        <v>81</v>
-      </c>
-    </row>
-    <row r="7" spans="1:37">
-      <c r="A7" t="s">
-        <v>118</v>
-      </c>
-      <c r="C7" s="1" t="s">
-        <v>149</v>
-      </c>
-    </row>
-    <row r="8" spans="1:37">
-      <c r="A8" t="s">
-        <v>119</v>
-      </c>
-      <c r="C8" s="4" t="s">
-        <v>150</v>
-      </c>
-    </row>
-    <row r="9" spans="1:37">
-      <c r="A9" t="s">
-        <v>120</v>
-      </c>
-      <c r="B9" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="10" spans="1:37">
-      <c r="A10" t="s">
-        <v>121</v>
-      </c>
-      <c r="B10" t="s">
-        <v>74</v>
-      </c>
-    </row>
-    <row r="11" spans="1:37">
-      <c r="A11" t="s">
-        <v>122</v>
-      </c>
-      <c r="B11" t="s">
-        <v>30</v>
-      </c>
-    </row>
-    <row r="12" spans="1:37">
-      <c r="A12" t="s">
-        <v>123</v>
-      </c>
-      <c r="B12" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="13" spans="1:37">
-      <c r="A13" t="s">
-        <v>124</v>
-      </c>
-      <c r="B13" t="s">
-        <v>23</v>
-      </c>
-    </row>
-    <row r="14" spans="1:37">
-      <c r="A14" t="s">
-        <v>125</v>
-      </c>
-      <c r="C14" s="2" t="s">
-        <v>160</v>
-      </c>
-    </row>
-    <row r="15" spans="1:37">
-      <c r="A15" t="s">
-        <v>126</v>
-      </c>
-      <c r="C15" s="1" t="s">
-        <v>149</v>
-      </c>
-    </row>
-    <row r="16" spans="1:37">
-      <c r="A16" t="s">
-        <v>127</v>
-      </c>
-      <c r="C16" s="2" t="s">
-        <v>160</v>
-      </c>
-    </row>
-    <row r="17" spans="1:7">
-      <c r="A17" t="s">
-        <v>128</v>
-      </c>
-      <c r="B17" t="s">
-        <v>97</v>
-      </c>
-    </row>
-    <row r="18" spans="1:7">
-      <c r="A18" t="s">
+      <c r="H22" t="s">
+        <v>17</v>
+      </c>
+      <c r="I22" t="s">
+        <v>33</v>
+      </c>
+      <c r="J22" t="s">
+        <v>75</v>
+      </c>
+      <c r="M22">
+        <v>0.93200000000000005</v>
+      </c>
+    </row>
+    <row r="23" spans="1:13" x14ac:dyDescent="0.5">
+      <c r="A23" t="s">
         <v>129</v>
       </c>
-      <c r="B18" t="s">
-        <v>37</v>
-      </c>
-    </row>
-    <row r="19" spans="1:7">
-      <c r="A19" t="s">
+      <c r="C23" s="2" t="s">
+        <v>163</v>
+      </c>
+      <c r="H23">
+        <v>0.2068497</v>
+      </c>
+      <c r="I23">
+        <v>0.37033830000000001</v>
+      </c>
+      <c r="J23">
+        <v>0.42281200000000002</v>
+      </c>
+    </row>
+    <row r="24" spans="1:13" x14ac:dyDescent="0.5">
+      <c r="A24" t="s">
         <v>130</v>
       </c>
-      <c r="B19" t="s">
-        <v>36</v>
-      </c>
-    </row>
-    <row r="20" spans="1:7">
-      <c r="A20" t="s">
+      <c r="B24" t="s">
+        <v>42</v>
+      </c>
+      <c r="G24" t="s">
+        <v>156</v>
+      </c>
+      <c r="H24" t="s">
+        <v>157</v>
+      </c>
+      <c r="I24" t="s">
+        <v>20</v>
+      </c>
+      <c r="M24">
+        <v>0.90700000000000003</v>
+      </c>
+    </row>
+    <row r="25" spans="1:13" x14ac:dyDescent="0.5">
+      <c r="A25" t="s">
         <v>131</v>
       </c>
-      <c r="B20" t="s">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="21" spans="1:7">
-      <c r="A21" t="s">
+      <c r="B25" t="s">
+        <v>45</v>
+      </c>
+      <c r="H25">
+        <v>0.22818150000000001</v>
+      </c>
+      <c r="I25">
+        <v>0.77181840000000002</v>
+      </c>
+    </row>
+    <row r="26" spans="1:13" x14ac:dyDescent="0.5">
+      <c r="A26" t="s">
         <v>132</v>
       </c>
-      <c r="C21" s="2" t="s">
-        <v>160</v>
-      </c>
-    </row>
-    <row r="22" spans="1:7">
-      <c r="A22" t="s">
+      <c r="C26" s="2" t="s">
+        <v>163</v>
+      </c>
+      <c r="G26" s="5"/>
+    </row>
+    <row r="27" spans="1:13" x14ac:dyDescent="0.5">
+      <c r="A27" t="s">
         <v>133</v>
       </c>
-      <c r="C22" s="2" t="s">
-        <v>160</v>
-      </c>
-    </row>
-    <row r="23" spans="1:7">
-      <c r="A23" t="s">
+      <c r="C27" s="2" t="s">
+        <v>163</v>
+      </c>
+      <c r="G27" s="3"/>
+    </row>
+    <row r="28" spans="1:13" x14ac:dyDescent="0.5">
+      <c r="A28" t="s">
         <v>134</v>
       </c>
-      <c r="B23" t="s">
-        <v>45</v>
-      </c>
-    </row>
-    <row r="24" spans="1:7">
-      <c r="A24" t="s">
+      <c r="B28" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="29" spans="1:13" x14ac:dyDescent="0.5">
+      <c r="A29" t="s">
         <v>135</v>
       </c>
-      <c r="B24" t="s">
-        <v>48</v>
-      </c>
-    </row>
-    <row r="25" spans="1:7">
-      <c r="A25" t="s">
+      <c r="C29" s="1" t="s">
+        <v>145</v>
+      </c>
+    </row>
+    <row r="30" spans="1:13" x14ac:dyDescent="0.5">
+      <c r="A30" t="s">
         <v>136</v>
       </c>
-      <c r="C25" s="2" t="s">
-        <v>160</v>
-      </c>
-      <c r="G25" s="5"/>
-    </row>
-    <row r="26" spans="1:7">
-      <c r="A26" t="s">
+      <c r="B30" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="31" spans="1:13" x14ac:dyDescent="0.5">
+      <c r="A31" t="s">
         <v>137</v>
       </c>
-      <c r="C26" s="2" t="s">
-        <v>160</v>
-      </c>
-      <c r="G26" s="3"/>
-    </row>
-    <row r="27" spans="1:7">
-      <c r="A27" t="s">
+      <c r="C31" s="4" t="s">
+        <v>162</v>
+      </c>
+    </row>
+    <row r="32" spans="1:13" x14ac:dyDescent="0.5">
+      <c r="A32" t="s">
         <v>138</v>
       </c>
-      <c r="B27" t="s">
-        <v>61</v>
-      </c>
-    </row>
-    <row r="28" spans="1:7">
-      <c r="A28" t="s">
+      <c r="C32" s="4" t="s">
+        <v>162</v>
+      </c>
+    </row>
+    <row r="33" spans="1:5" x14ac:dyDescent="0.5">
+      <c r="A33" t="s">
         <v>139</v>
       </c>
-      <c r="C28" s="1" t="s">
-        <v>149</v>
-      </c>
-    </row>
-    <row r="29" spans="1:7">
-      <c r="A29" t="s">
+      <c r="C33" s="4" t="s">
+        <v>162</v>
+      </c>
+    </row>
+    <row r="34" spans="1:5" x14ac:dyDescent="0.5">
+      <c r="A34" t="s">
         <v>140</v>
       </c>
-      <c r="B29" t="s">
-        <v>64</v>
-      </c>
-    </row>
-    <row r="30" spans="1:7">
-      <c r="A30" t="s">
+      <c r="B34" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="35" spans="1:5" x14ac:dyDescent="0.5">
+      <c r="A35" t="s">
         <v>141</v>
       </c>
-      <c r="C30" s="4" t="s">
-        <v>150</v>
-      </c>
-    </row>
-    <row r="31" spans="1:7">
-      <c r="A31" t="s">
+      <c r="B35" t="s">
+        <v>146</v>
+      </c>
+      <c r="C35" t="s">
+        <v>146</v>
+      </c>
+      <c r="E35" t="s">
+        <v>147</v>
+      </c>
+    </row>
+    <row r="36" spans="1:5" x14ac:dyDescent="0.5">
+      <c r="A36" t="s">
         <v>142</v>
       </c>
-      <c r="C31" s="4" t="s">
-        <v>150</v>
-      </c>
-    </row>
-    <row r="32" spans="1:7">
-      <c r="A32" t="s">
+      <c r="C36" s="1" t="s">
+        <v>145</v>
+      </c>
+    </row>
+    <row r="37" spans="1:5" x14ac:dyDescent="0.5">
+      <c r="A37" t="s">
         <v>143</v>
       </c>
-      <c r="C32" s="4" t="s">
-        <v>150</v>
-      </c>
-    </row>
-    <row r="33" spans="1:5">
-      <c r="A33" t="s">
+      <c r="C37" s="1" t="s">
+        <v>145</v>
+      </c>
+    </row>
+    <row r="38" spans="1:5" x14ac:dyDescent="0.5">
+      <c r="A38" t="s">
         <v>144</v>
       </c>
-      <c r="B33" t="s">
-        <v>25</v>
-      </c>
-    </row>
-    <row r="34" spans="1:5">
-      <c r="A34" t="s">
+      <c r="C38" s="1" t="s">
         <v>145</v>
-      </c>
-      <c r="C34" t="s">
-        <v>151</v>
-      </c>
-      <c r="E34" t="s">
-        <v>152</v>
-      </c>
-    </row>
-    <row r="35" spans="1:5">
-      <c r="A35" t="s">
-        <v>146</v>
-      </c>
-      <c r="C35" s="1" t="s">
-        <v>149</v>
-      </c>
-    </row>
-    <row r="36" spans="1:5">
-      <c r="A36" t="s">
-        <v>147</v>
-      </c>
-      <c r="C36" s="1" t="s">
-        <v>149</v>
-      </c>
-    </row>
-    <row r="37" spans="1:5">
-      <c r="A37" t="s">
-        <v>148</v>
-      </c>
-      <c r="C37" s="1" t="s">
-        <v>149</v>
       </c>
     </row>
   </sheetData>
@@ -2448,32 +2935,32 @@
   <dimension ref="A1:G12"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="K43" sqref="K43"/>
+      <selection activeCell="I15" sqref="I15"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4"/>
+  <sheetFormatPr defaultRowHeight="14.1" x14ac:dyDescent="0.5"/>
   <sheetData>
-    <row r="1" spans="1:7">
+    <row r="1" spans="1:7" x14ac:dyDescent="0.5">
       <c r="A1" t="s">
-        <v>156</v>
+        <v>151</v>
       </c>
       <c r="B1" t="s">
-        <v>20</v>
+        <v>17</v>
       </c>
       <c r="C1" t="s">
-        <v>6</v>
+        <v>3</v>
       </c>
       <c r="D1" t="s">
-        <v>71</v>
+        <v>68</v>
       </c>
       <c r="F1" t="s">
-        <v>157</v>
+        <v>152</v>
       </c>
       <c r="G1">
         <v>0.98199999999999998</v>
       </c>
     </row>
-    <row r="2" spans="1:7">
+    <row r="2" spans="1:7" x14ac:dyDescent="0.5">
       <c r="B2">
         <v>0.43030590000000002</v>
       </c>
@@ -2484,24 +2971,24 @@
         <v>0.44028050000000002</v>
       </c>
     </row>
-    <row r="3" spans="1:7">
+    <row r="3" spans="1:7" x14ac:dyDescent="0.5">
       <c r="A3" t="s">
-        <v>158</v>
+        <v>153</v>
       </c>
       <c r="B3" t="s">
-        <v>6</v>
+        <v>3</v>
       </c>
       <c r="C3" t="s">
-        <v>11</v>
+        <v>8</v>
       </c>
       <c r="D3" t="s">
-        <v>71</v>
+        <v>68</v>
       </c>
       <c r="G3">
         <v>0.98299999999999998</v>
       </c>
     </row>
-    <row r="4" spans="1:7">
+    <row r="4" spans="1:7" x14ac:dyDescent="0.5">
       <c r="B4">
         <v>0.54020354000000004</v>
       </c>
@@ -2512,24 +2999,24 @@
         <v>8.5701319999999998E-2</v>
       </c>
     </row>
-    <row r="5" spans="1:7">
+    <row r="5" spans="1:7" x14ac:dyDescent="0.5">
       <c r="A5" t="s">
-        <v>159</v>
+        <v>154</v>
       </c>
       <c r="B5" t="s">
-        <v>20</v>
+        <v>17</v>
       </c>
       <c r="C5" t="s">
-        <v>6</v>
+        <v>3</v>
       </c>
       <c r="D5" t="s">
-        <v>11</v>
+        <v>8</v>
       </c>
       <c r="G5">
         <v>0.97399999999999998</v>
       </c>
     </row>
-    <row r="6" spans="1:7">
+    <row r="6" spans="1:7" x14ac:dyDescent="0.5">
       <c r="B6">
         <v>0.48259819999999998</v>
       </c>
@@ -2540,21 +3027,21 @@
         <v>0.2429789</v>
       </c>
     </row>
-    <row r="7" spans="1:7">
+    <row r="7" spans="1:7" x14ac:dyDescent="0.5">
       <c r="A7" t="s">
-        <v>137</v>
+        <v>133</v>
       </c>
       <c r="B7" t="s">
-        <v>36</v>
+        <v>33</v>
       </c>
       <c r="C7" t="s">
-        <v>74</v>
+        <v>71</v>
       </c>
       <c r="G7">
         <v>0.97199999999999998</v>
       </c>
     </row>
-    <row r="8" spans="1:7">
+    <row r="8" spans="1:7" x14ac:dyDescent="0.5">
       <c r="B8">
         <v>0.56460290000000002</v>
       </c>
@@ -2562,24 +3049,24 @@
         <v>0.43539709999999998</v>
       </c>
     </row>
-    <row r="9" spans="1:7">
+    <row r="9" spans="1:7" x14ac:dyDescent="0.5">
       <c r="A9" t="s">
-        <v>161</v>
+        <v>155</v>
       </c>
       <c r="B9" t="s">
-        <v>20</v>
+        <v>17</v>
       </c>
       <c r="C9" t="s">
-        <v>36</v>
+        <v>33</v>
       </c>
       <c r="D9" t="s">
-        <v>78</v>
+        <v>75</v>
       </c>
       <c r="G9">
         <v>0.93200000000000005</v>
       </c>
     </row>
-    <row r="10" spans="1:7">
+    <row r="10" spans="1:7" x14ac:dyDescent="0.5">
       <c r="B10">
         <v>0.2068497</v>
       </c>
@@ -2590,27 +3077,539 @@
         <v>0.42281200000000002</v>
       </c>
     </row>
-    <row r="11" spans="1:7">
+    <row r="11" spans="1:7" x14ac:dyDescent="0.5">
       <c r="A11" t="s">
-        <v>162</v>
+        <v>156</v>
       </c>
       <c r="B11" t="s">
-        <v>163</v>
+        <v>157</v>
       </c>
       <c r="C11" t="s">
-        <v>23</v>
+        <v>20</v>
       </c>
       <c r="G11">
         <v>0.90700000000000003</v>
       </c>
     </row>
-    <row r="12" spans="1:7">
+    <row r="12" spans="1:7" x14ac:dyDescent="0.5">
       <c r="B12">
         <v>0.22818150000000001</v>
       </c>
       <c r="C12">
         <v>0.77181840000000002</v>
       </c>
+    </row>
+  </sheetData>
+  <phoneticPr fontId="1" type="noConversion"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{78CEA1C5-32B3-4100-A3D5-F0C20FD35051}">
+  <dimension ref="A2:D42"/>
+  <sheetViews>
+    <sheetView topLeftCell="A19" workbookViewId="0">
+      <selection activeCell="A2" sqref="A2:C42"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.1" x14ac:dyDescent="0.5"/>
+  <cols>
+    <col min="1" max="1" width="8.1484375" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="25.44921875" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="6.1484375" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="10.84765625" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="2" spans="1:4" ht="14.7" x14ac:dyDescent="0.5">
+      <c r="A2" s="8" t="s">
+        <v>164</v>
+      </c>
+      <c r="B2" s="8" t="s">
+        <v>165</v>
+      </c>
+      <c r="C2" s="8" t="s">
+        <v>166</v>
+      </c>
+      <c r="D2" s="8"/>
+    </row>
+    <row r="3" spans="1:4" ht="14.7" x14ac:dyDescent="0.5">
+      <c r="A3" s="8" t="s">
+        <v>167</v>
+      </c>
+      <c r="B3" s="8" t="s">
+        <v>168</v>
+      </c>
+      <c r="C3" s="8" t="s">
+        <v>166</v>
+      </c>
+      <c r="D3" s="8"/>
+    </row>
+    <row r="4" spans="1:4" ht="14.7" x14ac:dyDescent="0.5">
+      <c r="A4" s="8" t="s">
+        <v>169</v>
+      </c>
+      <c r="B4" s="8" t="s">
+        <v>170</v>
+      </c>
+      <c r="C4" s="8" t="s">
+        <v>166</v>
+      </c>
+      <c r="D4" s="8"/>
+    </row>
+    <row r="5" spans="1:4" ht="14.7" x14ac:dyDescent="0.5">
+      <c r="A5" s="8" t="s">
+        <v>171</v>
+      </c>
+      <c r="B5" s="8" t="s">
+        <v>172</v>
+      </c>
+      <c r="C5" s="8" t="s">
+        <v>166</v>
+      </c>
+      <c r="D5" s="8"/>
+    </row>
+    <row r="6" spans="1:4" ht="14.7" x14ac:dyDescent="0.5">
+      <c r="A6" s="8" t="s">
+        <v>173</v>
+      </c>
+      <c r="B6" s="8" t="s">
+        <v>174</v>
+      </c>
+      <c r="C6" s="8" t="s">
+        <v>175</v>
+      </c>
+      <c r="D6" s="8"/>
+    </row>
+    <row r="7" spans="1:4" ht="14.7" x14ac:dyDescent="0.5">
+      <c r="A7" s="8" t="s">
+        <v>176</v>
+      </c>
+      <c r="B7" s="8" t="s">
+        <v>177</v>
+      </c>
+      <c r="C7" s="8" t="s">
+        <v>175</v>
+      </c>
+      <c r="D7" s="8"/>
+    </row>
+    <row r="8" spans="1:4" ht="14.7" x14ac:dyDescent="0.5">
+      <c r="A8" s="8" t="s">
+        <v>178</v>
+      </c>
+      <c r="B8" s="8" t="s">
+        <v>179</v>
+      </c>
+      <c r="C8" s="8" t="s">
+        <v>175</v>
+      </c>
+      <c r="D8" s="8"/>
+    </row>
+    <row r="9" spans="1:4" ht="14.7" x14ac:dyDescent="0.5">
+      <c r="A9" s="8" t="s">
+        <v>180</v>
+      </c>
+      <c r="B9" s="8" t="s">
+        <v>181</v>
+      </c>
+      <c r="C9" s="8" t="s">
+        <v>182</v>
+      </c>
+      <c r="D9" s="8"/>
+    </row>
+    <row r="10" spans="1:4" ht="14.7" x14ac:dyDescent="0.5">
+      <c r="A10" s="8" t="s">
+        <v>183</v>
+      </c>
+      <c r="B10" s="8" t="s">
+        <v>255</v>
+      </c>
+      <c r="C10" s="8" t="s">
+        <v>184</v>
+      </c>
+      <c r="D10" s="8"/>
+    </row>
+    <row r="11" spans="1:4" ht="14.7" x14ac:dyDescent="0.5">
+      <c r="A11" s="8" t="s">
+        <v>185</v>
+      </c>
+      <c r="B11" s="8" t="s">
+        <v>254</v>
+      </c>
+      <c r="C11" s="8" t="s">
+        <v>184</v>
+      </c>
+      <c r="D11" s="8"/>
+    </row>
+    <row r="12" spans="1:4" ht="14.7" x14ac:dyDescent="0.5">
+      <c r="A12" s="8" t="s">
+        <v>186</v>
+      </c>
+      <c r="B12" s="8" t="s">
+        <v>187</v>
+      </c>
+      <c r="C12" s="8" t="s">
+        <v>188</v>
+      </c>
+      <c r="D12" s="8"/>
+    </row>
+    <row r="13" spans="1:4" ht="14.7" x14ac:dyDescent="0.5">
+      <c r="A13" s="8" t="s">
+        <v>189</v>
+      </c>
+      <c r="B13" s="8" t="s">
+        <v>256</v>
+      </c>
+      <c r="C13" s="8" t="s">
+        <v>188</v>
+      </c>
+      <c r="D13" s="8"/>
+    </row>
+    <row r="14" spans="1:4" ht="14.7" x14ac:dyDescent="0.5">
+      <c r="A14" s="8" t="s">
+        <v>190</v>
+      </c>
+      <c r="B14" s="8" t="s">
+        <v>191</v>
+      </c>
+      <c r="C14" s="8" t="s">
+        <v>192</v>
+      </c>
+      <c r="D14" s="8"/>
+    </row>
+    <row r="15" spans="1:4" ht="14.7" x14ac:dyDescent="0.5">
+      <c r="A15" s="8" t="s">
+        <v>193</v>
+      </c>
+      <c r="B15" s="8" t="s">
+        <v>194</v>
+      </c>
+      <c r="C15" s="8" t="s">
+        <v>72</v>
+      </c>
+      <c r="D15" s="8"/>
+    </row>
+    <row r="16" spans="1:4" ht="14.7" x14ac:dyDescent="0.5">
+      <c r="A16" s="8" t="s">
+        <v>195</v>
+      </c>
+      <c r="B16" s="8" t="s">
+        <v>196</v>
+      </c>
+      <c r="C16" s="8" t="s">
+        <v>197</v>
+      </c>
+      <c r="D16" s="8"/>
+    </row>
+    <row r="17" spans="1:4" ht="14.7" x14ac:dyDescent="0.5">
+      <c r="A17" s="8" t="s">
+        <v>201</v>
+      </c>
+      <c r="B17" s="8" t="s">
+        <v>202</v>
+      </c>
+      <c r="C17" s="8" t="s">
+        <v>203</v>
+      </c>
+      <c r="D17" s="8"/>
+    </row>
+    <row r="18" spans="1:4" ht="14.7" x14ac:dyDescent="0.5">
+      <c r="A18" s="8" t="s">
+        <v>204</v>
+      </c>
+      <c r="B18" s="8" t="s">
+        <v>205</v>
+      </c>
+      <c r="C18" s="8" t="s">
+        <v>206</v>
+      </c>
+      <c r="D18" s="8"/>
+    </row>
+    <row r="19" spans="1:4" ht="14.7" x14ac:dyDescent="0.5">
+      <c r="A19" s="8" t="s">
+        <v>207</v>
+      </c>
+      <c r="B19" s="8" t="s">
+        <v>208</v>
+      </c>
+      <c r="C19" s="8" t="s">
+        <v>209</v>
+      </c>
+      <c r="D19" s="8"/>
+    </row>
+    <row r="20" spans="1:4" ht="14.7" x14ac:dyDescent="0.5">
+      <c r="A20" s="8" t="s">
+        <v>210</v>
+      </c>
+      <c r="B20" s="8" t="s">
+        <v>211</v>
+      </c>
+      <c r="C20" s="8" t="s">
+        <v>212</v>
+      </c>
+      <c r="D20" s="8"/>
+    </row>
+    <row r="21" spans="1:4" ht="14.7" x14ac:dyDescent="0.5">
+      <c r="A21" s="8" t="s">
+        <v>213</v>
+      </c>
+      <c r="B21" s="8" t="s">
+        <v>214</v>
+      </c>
+      <c r="C21" s="8" t="s">
+        <v>215</v>
+      </c>
+      <c r="D21" s="8"/>
+    </row>
+    <row r="22" spans="1:4" ht="14.7" x14ac:dyDescent="0.5">
+      <c r="A22" s="8" t="s">
+        <v>216</v>
+      </c>
+      <c r="B22" s="8" t="s">
+        <v>257</v>
+      </c>
+      <c r="C22" s="8" t="s">
+        <v>84</v>
+      </c>
+      <c r="D22" s="8"/>
+    </row>
+    <row r="23" spans="1:4" ht="14.7" x14ac:dyDescent="0.5">
+      <c r="A23" s="8" t="s">
+        <v>217</v>
+      </c>
+      <c r="B23" s="8" t="s">
+        <v>253</v>
+      </c>
+      <c r="C23" s="8" t="s">
+        <v>50</v>
+      </c>
+      <c r="D23" s="8"/>
+    </row>
+    <row r="24" spans="1:4" ht="14.7" x14ac:dyDescent="0.5">
+      <c r="A24" s="8" t="s">
+        <v>219</v>
+      </c>
+      <c r="B24" s="8" t="s">
+        <v>220</v>
+      </c>
+      <c r="C24" s="8" t="s">
+        <v>221</v>
+      </c>
+      <c r="D24" s="8"/>
+    </row>
+    <row r="25" spans="1:4" ht="14.7" x14ac:dyDescent="0.5">
+      <c r="A25" s="8" t="s">
+        <v>222</v>
+      </c>
+      <c r="B25" s="8" t="s">
+        <v>223</v>
+      </c>
+      <c r="C25" s="8" t="s">
+        <v>218</v>
+      </c>
+      <c r="D25" s="8"/>
+    </row>
+    <row r="26" spans="1:4" ht="14.7" x14ac:dyDescent="0.5">
+      <c r="A26" s="8" t="s">
+        <v>224</v>
+      </c>
+      <c r="B26" s="8" t="s">
+        <v>225</v>
+      </c>
+      <c r="C26" s="8" t="s">
+        <v>218</v>
+      </c>
+      <c r="D26" s="8"/>
+    </row>
+    <row r="27" spans="1:4" ht="14.7" x14ac:dyDescent="0.5">
+      <c r="A27" s="8" t="s">
+        <v>226</v>
+      </c>
+      <c r="B27" s="8" t="s">
+        <v>227</v>
+      </c>
+      <c r="C27" s="8" t="s">
+        <v>218</v>
+      </c>
+      <c r="D27" s="8"/>
+    </row>
+    <row r="28" spans="1:4" ht="14.7" x14ac:dyDescent="0.5">
+      <c r="A28" s="8" t="s">
+        <v>228</v>
+      </c>
+      <c r="B28" s="8" t="s">
+        <v>229</v>
+      </c>
+      <c r="C28" s="8" t="s">
+        <v>230</v>
+      </c>
+      <c r="D28" s="8"/>
+    </row>
+    <row r="29" spans="1:4" ht="14.7" x14ac:dyDescent="0.5">
+      <c r="A29" s="8" t="s">
+        <v>198</v>
+      </c>
+      <c r="B29" s="8" t="s">
+        <v>252</v>
+      </c>
+      <c r="C29" s="8" t="s">
+        <v>200</v>
+      </c>
+      <c r="D29" s="8"/>
+    </row>
+    <row r="30" spans="1:4" ht="14.7" x14ac:dyDescent="0.5">
+      <c r="A30" s="8" t="s">
+        <v>231</v>
+      </c>
+      <c r="B30" s="8" t="s">
+        <v>199</v>
+      </c>
+      <c r="C30" s="8" t="s">
+        <v>200</v>
+      </c>
+      <c r="D30" s="8"/>
+    </row>
+    <row r="31" spans="1:4" ht="14.7" x14ac:dyDescent="0.5">
+      <c r="A31" s="8" t="s">
+        <v>232</v>
+      </c>
+      <c r="B31" s="8" t="s">
+        <v>258</v>
+      </c>
+      <c r="C31" s="8" t="s">
+        <v>101</v>
+      </c>
+      <c r="D31" s="8"/>
+    </row>
+    <row r="32" spans="1:4" ht="14.7" x14ac:dyDescent="0.5">
+      <c r="A32" s="8" t="s">
+        <v>233</v>
+      </c>
+      <c r="B32" s="8" t="s">
+        <v>259</v>
+      </c>
+      <c r="C32" s="8" t="s">
+        <v>56</v>
+      </c>
+      <c r="D32" s="8"/>
+    </row>
+    <row r="33" spans="1:4" ht="14.7" x14ac:dyDescent="0.5">
+      <c r="A33" s="8" t="s">
+        <v>234</v>
+      </c>
+      <c r="B33" s="8" t="s">
+        <v>235</v>
+      </c>
+      <c r="C33" s="8" t="s">
+        <v>236</v>
+      </c>
+      <c r="D33" s="8"/>
+    </row>
+    <row r="34" spans="1:4" ht="14.7" x14ac:dyDescent="0.5">
+      <c r="A34" s="8" t="s">
+        <v>237</v>
+      </c>
+      <c r="B34" s="8" t="s">
+        <v>238</v>
+      </c>
+      <c r="C34" s="8" t="s">
+        <v>239</v>
+      </c>
+      <c r="D34" s="8"/>
+    </row>
+    <row r="35" spans="1:4" ht="14.7" x14ac:dyDescent="0.5">
+      <c r="A35" s="8" t="s">
+        <v>240</v>
+      </c>
+      <c r="B35" s="8" t="s">
+        <v>241</v>
+      </c>
+      <c r="C35" s="8" t="s">
+        <v>242</v>
+      </c>
+      <c r="D35" s="8"/>
+    </row>
+    <row r="36" spans="1:4" ht="14.7" x14ac:dyDescent="0.5">
+      <c r="A36" s="8" t="s">
+        <v>243</v>
+      </c>
+      <c r="B36" s="8" t="s">
+        <v>265</v>
+      </c>
+      <c r="C36" s="8" t="s">
+        <v>87</v>
+      </c>
+      <c r="D36" s="8"/>
+    </row>
+    <row r="37" spans="1:4" ht="14.7" x14ac:dyDescent="0.5">
+      <c r="A37" s="8" t="s">
+        <v>244</v>
+      </c>
+      <c r="B37" s="8" t="s">
+        <v>262</v>
+      </c>
+      <c r="C37" s="8" t="s">
+        <v>54</v>
+      </c>
+      <c r="D37" s="8"/>
+    </row>
+    <row r="38" spans="1:4" ht="14.7" x14ac:dyDescent="0.5">
+      <c r="A38" s="8" t="s">
+        <v>245</v>
+      </c>
+      <c r="B38" s="8" t="s">
+        <v>261</v>
+      </c>
+      <c r="C38" s="8" t="s">
+        <v>54</v>
+      </c>
+      <c r="D38" s="8"/>
+    </row>
+    <row r="39" spans="1:4" ht="14.7" x14ac:dyDescent="0.5">
+      <c r="A39" s="8" t="s">
+        <v>246</v>
+      </c>
+      <c r="B39" s="8" t="s">
+        <v>260</v>
+      </c>
+      <c r="C39" s="8" t="s">
+        <v>62</v>
+      </c>
+      <c r="D39" s="8"/>
+    </row>
+    <row r="40" spans="1:4" ht="14.7" x14ac:dyDescent="0.5">
+      <c r="A40" s="8" t="s">
+        <v>247</v>
+      </c>
+      <c r="B40" s="8" t="s">
+        <v>248</v>
+      </c>
+      <c r="C40" s="8" t="s">
+        <v>249</v>
+      </c>
+      <c r="D40" s="8"/>
+    </row>
+    <row r="41" spans="1:4" ht="14.7" x14ac:dyDescent="0.5">
+      <c r="A41" s="8" t="s">
+        <v>250</v>
+      </c>
+      <c r="B41" s="8" t="s">
+        <v>263</v>
+      </c>
+      <c r="C41" s="8" t="s">
+        <v>46</v>
+      </c>
+      <c r="D41" s="8"/>
+    </row>
+    <row r="42" spans="1:4" ht="14.7" x14ac:dyDescent="0.5">
+      <c r="A42" s="8" t="s">
+        <v>251</v>
+      </c>
+      <c r="B42" s="8" t="s">
+        <v>264</v>
+      </c>
+      <c r="C42" s="8"/>
+      <c r="D42" s="8"/>
     </row>
   </sheetData>
   <phoneticPr fontId="1" type="noConversion"/>

</xml_diff>